<commit_message>
bluetooth, tof sensor and imu works
</commit_message>
<xml_diff>
--- a/BluePill PinOut.xlsx
+++ b/BluePill PinOut.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ChibiStudio\workspace161\AirShip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ChibiStudio\workspace161\AirShip\ENGG1100AirShipChibiOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECC6AB62-18CA-452B-A615-E48A21A2DE24}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{02B4FCFA-AA2A-4CAD-A14C-C2693A39F51E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17760" xr2:uid="{957F4C29-8600-4810-8A82-DDED25F3C6B2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>A0</t>
   </si>
@@ -135,12 +135,6 @@
     <t>TIM1-0</t>
   </si>
   <si>
-    <t>TIM1-1</t>
-  </si>
-  <si>
-    <t>TIM1-2</t>
-  </si>
-  <si>
     <t>TIM1-3</t>
   </si>
   <si>
@@ -178,6 +172,54 @@
   </si>
   <si>
     <t>RX2</t>
+  </si>
+  <si>
+    <t>SDA1</t>
+  </si>
+  <si>
+    <t>SCL1</t>
+  </si>
+  <si>
+    <t>RangeSensor SCL</t>
+  </si>
+  <si>
+    <t>RangeSensor SDA</t>
+  </si>
+  <si>
+    <t>TX1</t>
+  </si>
+  <si>
+    <t>RX1</t>
+  </si>
+  <si>
+    <t>TIM3-2</t>
+  </si>
+  <si>
+    <t>TIM3-3</t>
+  </si>
+  <si>
+    <t>TOF RX</t>
+  </si>
+  <si>
+    <t>TOF TX</t>
+  </si>
+  <si>
+    <t>Bluetooth RX</t>
+  </si>
+  <si>
+    <t>Bluetooth TX</t>
+  </si>
+  <si>
+    <t>TX3</t>
+  </si>
+  <si>
+    <t>RX3</t>
+  </si>
+  <si>
+    <t>IMU RX</t>
+  </si>
+  <si>
+    <t>IMU TX</t>
   </si>
 </sst>
 </file>
@@ -242,8 +284,8 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>403225</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>903</xdr:rowOff>
     </xdr:to>
@@ -586,22 +628,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD09037-0BF1-4DE7-B074-9B24071BE09E}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -619,7 +661,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -627,7 +672,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -645,10 +693,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -656,10 +704,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -670,7 +718,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,10 +726,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +737,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -700,10 +748,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -721,82 +769,118 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>

</xml_diff>